<commit_message>
anz upload today - jopat
</commit_message>
<xml_diff>
--- a/ANZ.XLSX
+++ b/ANZ.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="289">
   <si>
     <t>P891</t>
   </si>
@@ -163,10 +163,82 @@
     <t>ROL</t>
   </si>
   <si>
-    <t>133798742</t>
-  </si>
-  <si>
-    <t>ST JOHN OF GOD HEALTH CARE</t>
+    <t>133802469</t>
+  </si>
+  <si>
+    <t>WAURN PONDS DIAGNOSTIC IMAGING</t>
+  </si>
+  <si>
+    <t>03250768</t>
+  </si>
+  <si>
+    <t>PRIMOVIST SOLU PFS 1X10ML AU-NZ</t>
+  </si>
+  <si>
+    <t>2020724</t>
+  </si>
+  <si>
+    <t>HIGHTON</t>
+  </si>
+  <si>
+    <t>717069428</t>
+  </si>
+  <si>
+    <t>010050</t>
+  </si>
+  <si>
+    <t>133803107</t>
+  </si>
+  <si>
+    <t>SOUTHERN CROSS MEDICAL IMAGING</t>
+  </si>
+  <si>
+    <t>82212737</t>
+  </si>
+  <si>
+    <t>BILISCOPIN SOLU BT 1x100 ml AU NZ</t>
+  </si>
+  <si>
+    <t>3017936</t>
+  </si>
+  <si>
+    <t>BUNDOORA</t>
+  </si>
+  <si>
+    <t>717070721</t>
+  </si>
+  <si>
+    <t>133786713</t>
+  </si>
+  <si>
+    <t>ROYAL PRINCE ALFRED HOSPITAL</t>
+  </si>
+  <si>
+    <t>4595846</t>
+  </si>
+  <si>
+    <t>CAMPERDOWN</t>
+  </si>
+  <si>
+    <t>717066699</t>
+  </si>
+  <si>
+    <t>010130</t>
+  </si>
+  <si>
+    <t>4595817</t>
+  </si>
+  <si>
+    <t>SYDNEY LOCAL HEALTH DISTRICT OU</t>
+  </si>
+  <si>
+    <t>PARRAMATTA</t>
+  </si>
+  <si>
+    <t>133786714</t>
+  </si>
+  <si>
+    <t>AUBURN HOSPITAL</t>
   </si>
   <si>
     <t>80727543</t>
@@ -175,46 +247,34 @@
     <t>UROGRAFIN 30% SOLU AMPO 10x10ml AU</t>
   </si>
   <si>
-    <t>3018198</t>
-  </si>
-  <si>
-    <t>WENDOUREE VILLAGE</t>
-  </si>
-  <si>
-    <t>717069811</t>
-  </si>
-  <si>
-    <t>020050</t>
-  </si>
-  <si>
-    <t>133802469</t>
-  </si>
-  <si>
-    <t>WAURN PONDS DIAGNOSTIC IMAGING</t>
-  </si>
-  <si>
-    <t>03250768</t>
-  </si>
-  <si>
-    <t>PRIMOVIST SOLU PFS 1X10ML AU-NZ</t>
-  </si>
-  <si>
-    <t>2020724</t>
-  </si>
-  <si>
-    <t>HIGHTON</t>
-  </si>
-  <si>
-    <t>717069428</t>
-  </si>
-  <si>
-    <t>010050</t>
-  </si>
-  <si>
-    <t>133805269</t>
-  </si>
-  <si>
-    <t>QSCAN RADIOLOGY CLINIC - TOOWONG</t>
+    <t>4596110</t>
+  </si>
+  <si>
+    <t>AUBURN</t>
+  </si>
+  <si>
+    <t>717066995</t>
+  </si>
+  <si>
+    <t>4596108</t>
+  </si>
+  <si>
+    <t>WESTERN SYDNEY LOCAL HEALTH DISTRIC</t>
+  </si>
+  <si>
+    <t>133786715</t>
+  </si>
+  <si>
+    <t>4595813</t>
+  </si>
+  <si>
+    <t>717068742</t>
+  </si>
+  <si>
+    <t>133796060</t>
+  </si>
+  <si>
+    <t>PRP Diagnostic Imaging - Zetland</t>
   </si>
   <si>
     <t>80802544</t>
@@ -223,13 +283,259 @@
     <t>GADOVIST 1.0 SOLU PFS 5X5ML AU-NZ</t>
   </si>
   <si>
-    <t>3320238</t>
-  </si>
-  <si>
-    <t>TOOWONG</t>
-  </si>
-  <si>
-    <t>717067377</t>
+    <t>776826</t>
+  </si>
+  <si>
+    <t>Zetland</t>
+  </si>
+  <si>
+    <t>717068849</t>
+  </si>
+  <si>
+    <t>4595823</t>
+  </si>
+  <si>
+    <t>PRP DIAGNOSTIC IMAGING</t>
+  </si>
+  <si>
+    <t>GOSFORD</t>
+  </si>
+  <si>
+    <t>133796062</t>
+  </si>
+  <si>
+    <t>VISION RADIOLOGY RESERVIOR</t>
+  </si>
+  <si>
+    <t>963299</t>
+  </si>
+  <si>
+    <t>RESERVIOR</t>
+  </si>
+  <si>
+    <t>717070377</t>
+  </si>
+  <si>
+    <t>133799462</t>
+  </si>
+  <si>
+    <t>BELMONT DISTRICT HOSPITAL</t>
+  </si>
+  <si>
+    <t>4595240</t>
+  </si>
+  <si>
+    <t>BELMONT</t>
+  </si>
+  <si>
+    <t>717071400</t>
+  </si>
+  <si>
+    <t>4595328</t>
+  </si>
+  <si>
+    <t>HUNTER NEW ENGLAND LOCAL HEALTH DIS</t>
+  </si>
+  <si>
+    <t>NEWCASTLE</t>
+  </si>
+  <si>
+    <t>133801040</t>
+  </si>
+  <si>
+    <t>THE RADIOLOGY CLINIC PTY LTD</t>
+  </si>
+  <si>
+    <t>86698188</t>
+  </si>
+  <si>
+    <t>STLNT,KIT,SYR,CT,DUAL,TCON,SPK,MC,WLD</t>
+  </si>
+  <si>
+    <t>4614735</t>
+  </si>
+  <si>
+    <t>MAROOCHYDORE</t>
+  </si>
+  <si>
+    <t>717057868</t>
+  </si>
+  <si>
+    <t>87078760</t>
+  </si>
+  <si>
+    <t>STLNT,KIT,SYR,CT,S,SPK,FLS3,150ML,WLD</t>
+  </si>
+  <si>
+    <t>133802065</t>
+  </si>
+  <si>
+    <t>CAMPBELLTOWN HOSPITAL</t>
+  </si>
+  <si>
+    <t>4596093</t>
+  </si>
+  <si>
+    <t>CAMPBELLTOWN</t>
+  </si>
+  <si>
+    <t>717066697</t>
+  </si>
+  <si>
+    <t>4596097</t>
+  </si>
+  <si>
+    <t>SOUTH WESTERN SYDNEY LOCAL HEALTH D</t>
+  </si>
+  <si>
+    <t>133802250</t>
+  </si>
+  <si>
+    <t>JONES RADIOLOGY - ST ANDREW'S</t>
+  </si>
+  <si>
+    <t>88320468</t>
+  </si>
+  <si>
+    <t>DOTAGRAF SOLU BT 10X100ML AU</t>
+  </si>
+  <si>
+    <t>4595373</t>
+  </si>
+  <si>
+    <t>ADELAIDE</t>
+  </si>
+  <si>
+    <t>717065584</t>
+  </si>
+  <si>
+    <t>133802251</t>
+  </si>
+  <si>
+    <t>ACT HEALTH SUPPLY SERVICES - THE</t>
+  </si>
+  <si>
+    <t>4595648</t>
+  </si>
+  <si>
+    <t>BRUCE</t>
+  </si>
+  <si>
+    <t>717068823</t>
+  </si>
+  <si>
+    <t>4595647</t>
+  </si>
+  <si>
+    <t>ACT HEALTH SUPPLY SERVICES</t>
+  </si>
+  <si>
+    <t>MITCHELL</t>
+  </si>
+  <si>
+    <t>133802252</t>
+  </si>
+  <si>
+    <t>I-Med Fortitude Valley</t>
+  </si>
+  <si>
+    <t>778888</t>
+  </si>
+  <si>
+    <t>Fortitude Valley</t>
+  </si>
+  <si>
+    <t>717071342</t>
+  </si>
+  <si>
+    <t>133802253</t>
+  </si>
+  <si>
+    <t>I-MED RADIOLOGY - PENINSULA PH</t>
+  </si>
+  <si>
+    <t>86594218</t>
+  </si>
+  <si>
+    <t>SOLARIS,KIT,SYR,MRI,65/115ML,MC,WLD</t>
+  </si>
+  <si>
+    <t>4595941</t>
+  </si>
+  <si>
+    <t>FRANKSTON</t>
+  </si>
+  <si>
+    <t>717071461</t>
+  </si>
+  <si>
+    <t>86698242</t>
+  </si>
+  <si>
+    <t>STLNT,KIT,SYR,CT,SNGL,60",SPK,MC,WLD</t>
+  </si>
+  <si>
+    <t>86610280</t>
+  </si>
+  <si>
+    <t>ASSY,TUBE SET,STELLANT MP,MIC,MC,EU</t>
+  </si>
+  <si>
+    <t>133803010</t>
+  </si>
+  <si>
+    <t>LAKE IMAGING - BALLARAT</t>
+  </si>
+  <si>
+    <t>64424260</t>
+  </si>
+  <si>
+    <t>LabEAZY Cassette- 68Ga PSMA Peptides</t>
+  </si>
+  <si>
+    <t>4595977</t>
+  </si>
+  <si>
+    <t>BALLARAT</t>
+  </si>
+  <si>
+    <t>717066625</t>
+  </si>
+  <si>
+    <t>4595969</t>
+  </si>
+  <si>
+    <t>LAKE IMAGING PTY LTD</t>
+  </si>
+  <si>
+    <t>GEELONG</t>
+  </si>
+  <si>
+    <t>64424244</t>
+  </si>
+  <si>
+    <t>LabEAZY Cassette- 68Ga DOTA Peptides</t>
+  </si>
+  <si>
+    <t>133805151</t>
+  </si>
+  <si>
+    <t>UNIVERSAL MEDICAL IMAGING -  BRUCE</t>
+  </si>
+  <si>
+    <t>4595749</t>
+  </si>
+  <si>
+    <t>717068565</t>
+  </si>
+  <si>
+    <t>4595747</t>
+  </si>
+  <si>
+    <t>UNIVERSAL MEDICAL IMAGING</t>
+  </si>
+  <si>
+    <t>CLAYFIELD</t>
   </si>
   <si>
     <t>02112548</t>
@@ -238,205 +544,133 @@
     <t>GADOVIST 1.0 SOLU PFS 5X7.5ML AU-NZ</t>
   </si>
   <si>
-    <t>87621529</t>
-  </si>
-  <si>
-    <t>GADOVIST 1.0 SOLU PFS 5X10ML AU-NZ</t>
-  </si>
-  <si>
-    <t>133786713</t>
-  </si>
-  <si>
-    <t>ROYAL PRINCE ALFRED HOSPITAL</t>
-  </si>
-  <si>
-    <t>4595846</t>
-  </si>
-  <si>
-    <t>CAMPERDOWN</t>
-  </si>
-  <si>
-    <t>717066699</t>
-  </si>
-  <si>
-    <t>010130</t>
-  </si>
-  <si>
-    <t>4595817</t>
-  </si>
-  <si>
-    <t>SYDNEY LOCAL HEALTH DISTRICT OU</t>
-  </si>
-  <si>
-    <t>PARRAMATTA</t>
-  </si>
-  <si>
-    <t>133786714</t>
-  </si>
-  <si>
-    <t>AUBURN HOSPITAL</t>
-  </si>
-  <si>
-    <t>4596110</t>
-  </si>
-  <si>
-    <t>AUBURN</t>
-  </si>
-  <si>
-    <t>717066995</t>
-  </si>
-  <si>
-    <t>4596108</t>
-  </si>
-  <si>
-    <t>WESTERN SYDNEY LOCAL HEALTH DISTRIC</t>
-  </si>
-  <si>
-    <t>133786715</t>
-  </si>
-  <si>
-    <t>4595813</t>
-  </si>
-  <si>
-    <t>717068742</t>
-  </si>
-  <si>
-    <t>133786716</t>
-  </si>
-  <si>
-    <t>NORTHEAST HEALTH WANGARATTA</t>
-  </si>
-  <si>
-    <t>4595865</t>
-  </si>
-  <si>
-    <t>WANGARATTA</t>
-  </si>
-  <si>
-    <t>717070710</t>
-  </si>
-  <si>
-    <t>4595866</t>
-  </si>
-  <si>
-    <t>133800647</t>
-  </si>
-  <si>
-    <t>GOSFORD HOSPITAL</t>
-  </si>
-  <si>
-    <t>4595426</t>
-  </si>
-  <si>
-    <t>GOSFORD</t>
-  </si>
-  <si>
-    <t>717070560</t>
-  </si>
-  <si>
-    <t>4595430</t>
-  </si>
-  <si>
-    <t>CENTRAL COAST LOCAL HEALTH</t>
+    <t>133805508</t>
+  </si>
+  <si>
+    <t>CONS ROBINA HOSPITAL OAO-0G0-652</t>
+  </si>
+  <si>
+    <t>02112555</t>
+  </si>
+  <si>
+    <t>GADOVIST 1.0 SOLU VIAL 10X15ML AU-NZ</t>
+  </si>
+  <si>
+    <t>971721</t>
+  </si>
+  <si>
+    <t>ROBINA</t>
+  </si>
+  <si>
+    <t>717070451</t>
+  </si>
+  <si>
+    <t>4595661</t>
+  </si>
+  <si>
+    <t>GOLD COAST HOSPITAL &amp; HEALTH</t>
+  </si>
+  <si>
+    <t>SOUTHPORT</t>
+  </si>
+  <si>
+    <t>133805578</t>
+  </si>
+  <si>
+    <t>THE CANBERRA HOSPITAL</t>
+  </si>
+  <si>
+    <t>4595653</t>
+  </si>
+  <si>
+    <t>GARRAN</t>
+  </si>
+  <si>
+    <t>717067249</t>
+  </si>
+  <si>
+    <t>133805583</t>
+  </si>
+  <si>
+    <t>4595811</t>
+  </si>
+  <si>
+    <t>717068555</t>
+  </si>
+  <si>
+    <t>133805585</t>
+  </si>
+  <si>
+    <t>TOOWOOMBA HOSPITAL</t>
+  </si>
+  <si>
+    <t>4595344</t>
+  </si>
+  <si>
+    <t>TOOWOOMBA</t>
+  </si>
+  <si>
+    <t>717070603</t>
+  </si>
+  <si>
+    <t>4595342</t>
+  </si>
+  <si>
+    <t>DARLING DOWNS HOSPITAL &amp;</t>
+  </si>
+  <si>
+    <t>133805840</t>
+  </si>
+  <si>
+    <t>I-MED RADIOLOGY - SMRI</t>
+  </si>
+  <si>
+    <t>4658360</t>
+  </si>
+  <si>
+    <t>NEWTOWN</t>
+  </si>
+  <si>
+    <t>717063566</t>
+  </si>
+  <si>
+    <t>133805841</t>
+  </si>
+  <si>
+    <t>COFFS HARBOUR HOSPITAL</t>
+  </si>
+  <si>
+    <t>4595214</t>
+  </si>
+  <si>
+    <t>COFFS HARBOUR</t>
+  </si>
+  <si>
+    <t>717067136</t>
+  </si>
+  <si>
+    <t>4595220</t>
+  </si>
+  <si>
+    <t>MID NORTH COAST LOCAL HEALTH DISTRI</t>
   </si>
   <si>
     <t>HUNTER REGION MAIL CENTRE</t>
   </si>
   <si>
-    <t>133802065</t>
-  </si>
-  <si>
-    <t>CAMPBELLTOWN HOSPITAL</t>
-  </si>
-  <si>
-    <t>4596093</t>
-  </si>
-  <si>
-    <t>CAMPBELLTOWN</t>
-  </si>
-  <si>
-    <t>717066697</t>
-  </si>
-  <si>
-    <t>4596097</t>
-  </si>
-  <si>
-    <t>SOUTH WESTERN SYDNEY LOCAL HEALTH D</t>
-  </si>
-  <si>
-    <t>133802385</t>
-  </si>
-  <si>
-    <t>AUSTIN HEALTH  - VERNON AVE</t>
-  </si>
-  <si>
-    <t>4595496</t>
-  </si>
-  <si>
-    <t>HEIDELBERG WEST</t>
-  </si>
-  <si>
-    <t>717068897</t>
-  </si>
-  <si>
-    <t>4595508</t>
-  </si>
-  <si>
-    <t>AUSTIN HEALTH - FINANCE DEPT</t>
-  </si>
-  <si>
-    <t>HEIDELBERG</t>
-  </si>
-  <si>
-    <t>133802386</t>
-  </si>
-  <si>
-    <t>QUEENSLAND DIAGNOSTIC IMAGING</t>
-  </si>
-  <si>
-    <t>87238504</t>
-  </si>
-  <si>
-    <t>TUBE,EXT,SINGLE,WLD1</t>
-  </si>
-  <si>
-    <t>4595637</t>
-  </si>
-  <si>
-    <t>BRISBANE</t>
-  </si>
-  <si>
-    <t>717069166</t>
-  </si>
-  <si>
-    <t>4595468</t>
-  </si>
-  <si>
-    <t>QLD DIAGNOSTIC IMAGING PTY LTD</t>
-  </si>
-  <si>
-    <t>ST LEONARDS</t>
-  </si>
-  <si>
-    <t>133802387</t>
+    <t>133805842</t>
   </si>
   <si>
     <t>ST VINCENTS HOSPITAL SYDNEY</t>
   </si>
   <si>
-    <t>86698242</t>
-  </si>
-  <si>
-    <t>STLNT,KIT,SYR,CT,SNGL,60",SPK,MC,WLD</t>
-  </si>
-  <si>
     <t>4595515</t>
   </si>
   <si>
     <t>DARLINGHURST</t>
   </si>
   <si>
-    <t>717069842</t>
+    <t>717067306</t>
   </si>
   <si>
     <t>4595511</t>
@@ -445,142 +679,58 @@
     <t>ST VINCENT'S HOSPITAL SYDNEY LTD</t>
   </si>
   <si>
-    <t>133805270</t>
-  </si>
-  <si>
-    <t>QSCAN KINGSTON</t>
-  </si>
-  <si>
-    <t>4595740</t>
-  </si>
-  <si>
-    <t>KINGSTON</t>
-  </si>
-  <si>
-    <t>717069426</t>
-  </si>
-  <si>
-    <t>4595747</t>
-  </si>
-  <si>
-    <t>UNIVERSAL MEDICAL IMAGING</t>
-  </si>
-  <si>
-    <t>CLAYFIELD</t>
-  </si>
-  <si>
-    <t>133805348</t>
-  </si>
-  <si>
-    <t>i-MED RADIOLOGY - CASEY</t>
-  </si>
-  <si>
-    <t>86610280</t>
-  </si>
-  <si>
-    <t>ASSY,TUBE SET,STELLANT MP,MIC,MC,EU</t>
-  </si>
-  <si>
-    <t>4595719</t>
-  </si>
-  <si>
-    <t>BERWICK</t>
-  </si>
-  <si>
-    <t>717069429</t>
-  </si>
-  <si>
-    <t>133805351</t>
-  </si>
-  <si>
-    <t>02112555</t>
-  </si>
-  <si>
-    <t>GADOVIST 1.0 SOLU VIAL 10X15ML AU-NZ</t>
-  </si>
-  <si>
-    <t>717070393</t>
-  </si>
-  <si>
-    <t>133805352</t>
-  </si>
-  <si>
-    <t>717070551</t>
-  </si>
-  <si>
-    <t>133805508</t>
-  </si>
-  <si>
-    <t>CONS ROBINA HOSPITAL OAO-0G0-652</t>
-  </si>
-  <si>
-    <t>971721</t>
-  </si>
-  <si>
-    <t>ROBINA</t>
-  </si>
-  <si>
-    <t>717070451</t>
-  </si>
-  <si>
-    <t>4595661</t>
-  </si>
-  <si>
-    <t>GOLD COAST HOSPITAL &amp; HEALTH</t>
-  </si>
-  <si>
-    <t>SOUTHPORT</t>
-  </si>
-  <si>
-    <t>133679913</t>
-  </si>
-  <si>
-    <t>ROYAL PERTH HOSPITAL</t>
-  </si>
-  <si>
-    <t>4595756</t>
-  </si>
-  <si>
-    <t>PERTH</t>
-  </si>
-  <si>
-    <t>717070410</t>
+    <t>133695973</t>
+  </si>
+  <si>
+    <t>64050719</t>
+  </si>
+  <si>
+    <t>ULTRAVIST 370 SOLU BT 10X100ML AU-NZ</t>
+  </si>
+  <si>
+    <t>717066598</t>
+  </si>
+  <si>
+    <t>00658781</t>
+  </si>
+  <si>
+    <t>ULTRAVIST 370 SOLU BT 1X200ML AU</t>
+  </si>
+  <si>
+    <t>133805843</t>
+  </si>
+  <si>
+    <t>APEX RADIOLOGY - MANDURAH</t>
+  </si>
+  <si>
+    <t>3605378</t>
+  </si>
+  <si>
+    <t>MANDURAH</t>
+  </si>
+  <si>
+    <t>717070562</t>
   </si>
   <si>
     <t>010530</t>
   </si>
   <si>
-    <t>4595766</t>
-  </si>
-  <si>
-    <t>DEPARTMENT OF HEALTH WA</t>
-  </si>
-  <si>
-    <t>RAILWAY ROAD</t>
-  </si>
-  <si>
-    <t>133805268</t>
-  </si>
-  <si>
-    <t>PERTH RAD CLINIC LTD - SJOG MIDLAND</t>
-  </si>
-  <si>
-    <t>4595281</t>
-  </si>
-  <si>
-    <t>MIDLAND</t>
-  </si>
-  <si>
-    <t>717067376</t>
-  </si>
-  <si>
-    <t>4595291</t>
-  </si>
-  <si>
-    <t>PERTHRADCLINIC LTD</t>
-  </si>
-  <si>
-    <t>MIRRABOOKA</t>
+    <t>4596050</t>
+  </si>
+  <si>
+    <t>APEX RADIOLOGY</t>
+  </si>
+  <si>
+    <t>133805899</t>
+  </si>
+  <si>
+    <t>APEX RADIOLOGY - PEEL SPECIALIST</t>
+  </si>
+  <si>
+    <t>4596049</t>
+  </si>
+  <si>
+    <t>717071431</t>
   </si>
   <si>
     <t>P8SW</t>
@@ -644,18 +794,6 @@
   </si>
   <si>
     <t>2172497900</t>
-  </si>
-  <si>
-    <t>133786056</t>
-  </si>
-  <si>
-    <t>60727838</t>
-  </si>
-  <si>
-    <t>ASSY,DISPLAY,PHOENIX,STELLANT</t>
-  </si>
-  <si>
-    <t>2172549316</t>
   </si>
   <si>
     <t>133805528</t>
@@ -844,7 +982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -854,7 +992,7 @@
   <cols>
     <col min="1" max="1" bestFit="1" width="18" customWidth="1"/>
     <col min="2" max="2" bestFit="1" width="11" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="37" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="36" customWidth="1"/>
     <col min="4" max="4" bestFit="1" width="14" customWidth="1"/>
     <col min="5" max="5" bestFit="1" width="10" customWidth="1"/>
     <col min="6" max="6" bestFit="1" width="41" customWidth="1"/>
@@ -863,7 +1001,7 @@
     <col min="9" max="9" bestFit="1" width="14" customWidth="1"/>
     <col min="10" max="10" bestFit="1" width="6" customWidth="1"/>
     <col min="11" max="11" bestFit="1" width="15" customWidth="1"/>
-    <col min="12" max="12" bestFit="1" width="19" customWidth="1"/>
+    <col min="12" max="12" bestFit="1" width="18" customWidth="1"/>
     <col min="13" max="13" bestFit="1" width="15" customWidth="1"/>
     <col min="14" max="14" bestFit="1" width="6" customWidth="1"/>
     <col min="15" max="15" bestFit="1" width="21" customWidth="1"/>
@@ -880,76 +1018,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="4" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>268</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>232</v>
+        <v>278</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>233</v>
+        <v>279</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>234</v>
+        <v>280</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>235</v>
+        <v>281</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>236</v>
+        <v>282</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>239</v>
+        <v>285</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>240</v>
+        <v>286</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -1638,10 +1776,10 @@
         <v>53</v>
       </c>
       <c r="G11" s="3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H11" s="3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I11" t="s">
         <v>5</v>
@@ -1671,7 +1809,7 @@
         <v>45405</v>
       </c>
       <c r="R11" s="2">
-        <v>45408</v>
+        <v>45406</v>
       </c>
       <c r="S11" t="s">
         <v>57</v>
@@ -1712,10 +1850,10 @@
         <v>61</v>
       </c>
       <c r="G12" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I12" t="s">
         <v>5</v>
@@ -1748,7 +1886,7 @@
         <v>45406</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="T12" t="s">
         <v>62</v>
@@ -1771,25 +1909,25 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
       <c r="D13" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="G13" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" t="s">
         <v>5</v>
@@ -1798,10 +1936,10 @@
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M13" t="s">
         <v>9</v>
@@ -1810,28 +1948,28 @@
         <v>10</v>
       </c>
       <c r="O13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P13" t="s">
         <v>30</v>
       </c>
       <c r="Q13" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="R13" s="2">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="S13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="T13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="V13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W13" t="s">
         <v>14</v>
@@ -1845,25 +1983,25 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G14" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H14" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I14" t="s">
         <v>5</v>
@@ -1872,10 +2010,10 @@
         <v>6</v>
       </c>
       <c r="K14" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="L14" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="M14" t="s">
         <v>9</v>
@@ -1884,28 +2022,28 @@
         <v>10</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="P14" t="s">
         <v>30</v>
       </c>
       <c r="Q14" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="R14" s="2">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="S14" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="T14" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="U14" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="V14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W14" t="s">
         <v>14</v>
@@ -1919,25 +2057,25 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
       <c r="D15" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="G15" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H15" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -1946,10 +2084,10 @@
         <v>6</v>
       </c>
       <c r="K15" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="L15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M15" t="s">
         <v>9</v>
@@ -1958,28 +2096,28 @@
         <v>10</v>
       </c>
       <c r="O15" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
         <v>30</v>
       </c>
       <c r="Q15" s="2">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="R15" s="2">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="S15" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="T15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U15" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="V15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W15" t="s">
         <v>14</v>
@@ -1993,25 +2131,25 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2">
         <v>45406</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="G16" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I16" t="s">
         <v>5</v>
@@ -2020,10 +2158,10 @@
         <v>6</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="L16" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="M16" t="s">
         <v>9</v>
@@ -2032,7 +2170,7 @@
         <v>10</v>
       </c>
       <c r="O16" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="P16" t="s">
         <v>30</v>
@@ -2044,16 +2182,16 @@
         <v>45408</v>
       </c>
       <c r="S16" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T16" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="U16" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="V16" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="W16" t="s">
         <v>14</v>
@@ -2067,10 +2205,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2">
         <v>45406</v>
@@ -2082,10 +2220,10 @@
         <v>53</v>
       </c>
       <c r="G17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17" t="s">
         <v>5</v>
@@ -2094,10 +2232,10 @@
         <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="L17" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="M17" t="s">
         <v>9</v>
@@ -2106,7 +2244,7 @@
         <v>10</v>
       </c>
       <c r="O17" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="P17" t="s">
         <v>30</v>
@@ -2118,16 +2256,16 @@
         <v>45408</v>
       </c>
       <c r="S17" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T17" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="U17" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="V17" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="W17" t="s">
         <v>14</v>
@@ -2141,10 +2279,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D18" s="2">
         <v>45406</v>
@@ -2156,10 +2294,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H18" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
         <v>5</v>
@@ -2168,10 +2306,10 @@
         <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="L18" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="M18" t="s">
         <v>9</v>
@@ -2180,7 +2318,7 @@
         <v>10</v>
       </c>
       <c r="O18" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="P18" t="s">
         <v>30</v>
@@ -2192,16 +2330,16 @@
         <v>45408</v>
       </c>
       <c r="S18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T18" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="U18" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="V18" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="W18" t="s">
         <v>14</v>
@@ -2215,25 +2353,25 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D19" s="2">
         <v>45406</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="G19" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I19" t="s">
         <v>5</v>
@@ -2242,10 +2380,10 @@
         <v>6</v>
       </c>
       <c r="K19" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="L19" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="M19" t="s">
         <v>9</v>
@@ -2254,7 +2392,7 @@
         <v>10</v>
       </c>
       <c r="O19" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="P19" t="s">
         <v>30</v>
@@ -2269,13 +2407,13 @@
         <v>13</v>
       </c>
       <c r="T19" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="U19" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="V19" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="W19" t="s">
         <v>14</v>
@@ -2289,25 +2427,25 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2">
         <v>45406</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="G20" s="3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="H20" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
         <v>5</v>
@@ -2316,10 +2454,10 @@
         <v>6</v>
       </c>
       <c r="K20" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="L20" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="M20" t="s">
         <v>9</v>
@@ -2328,7 +2466,7 @@
         <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
@@ -2343,13 +2481,13 @@
         <v>13</v>
       </c>
       <c r="T20" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="U20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="V20" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="W20" t="s">
         <v>14</v>
@@ -2363,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D21" s="2">
         <v>45406</v>
@@ -2390,10 +2528,10 @@
         <v>6</v>
       </c>
       <c r="K21" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="L21" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="M21" t="s">
         <v>9</v>
@@ -2402,7 +2540,7 @@
         <v>10</v>
       </c>
       <c r="O21" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="P21" t="s">
         <v>30</v>
@@ -2414,16 +2552,16 @@
         <v>45408</v>
       </c>
       <c r="S21" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T21" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="U21" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="V21" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="W21" t="s">
         <v>14</v>
@@ -2437,25 +2575,25 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D22" s="2">
         <v>45406</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="G22" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H22" s="3">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="I22" t="s">
         <v>5</v>
@@ -2464,10 +2602,10 @@
         <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="L22" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="M22" t="s">
         <v>9</v>
@@ -2476,7 +2614,7 @@
         <v>10</v>
       </c>
       <c r="O22" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="P22" t="s">
         <v>30</v>
@@ -2485,19 +2623,19 @@
         <v>45406</v>
       </c>
       <c r="R22" s="2">
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="S22" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="T22" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="U22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="V22" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="W22" t="s">
         <v>14</v>
@@ -2511,25 +2649,25 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D23" s="2">
         <v>45406</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="G23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I23" t="s">
         <v>5</v>
@@ -2538,10 +2676,10 @@
         <v>6</v>
       </c>
       <c r="K23" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="L23" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="M23" t="s">
         <v>9</v>
@@ -2550,7 +2688,7 @@
         <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -2562,16 +2700,16 @@
         <v>45408</v>
       </c>
       <c r="S23" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T23" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="U23" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="V23" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="W23" t="s">
         <v>14</v>
@@ -2585,25 +2723,25 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D24" s="2">
         <v>45406</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="G24" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I24" t="s">
         <v>5</v>
@@ -2612,10 +2750,10 @@
         <v>6</v>
       </c>
       <c r="K24" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="L24" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M24" t="s">
         <v>9</v>
@@ -2624,7 +2762,7 @@
         <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="P24" t="s">
         <v>30</v>
@@ -2636,16 +2774,16 @@
         <v>45408</v>
       </c>
       <c r="S24" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T24" t="s">
         <v>142</v>
       </c>
       <c r="U24" t="s">
+        <v>141</v>
+      </c>
+      <c r="V24" t="s">
         <v>143</v>
-      </c>
-      <c r="V24" t="s">
-        <v>140</v>
       </c>
       <c r="W24" t="s">
         <v>14</v>
@@ -2659,25 +2797,25 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D25" s="2">
         <v>45406</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="G25" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H25" s="3">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I25" t="s">
         <v>5</v>
@@ -2686,10 +2824,10 @@
         <v>6</v>
       </c>
       <c r="K25" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="L25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="M25" t="s">
         <v>9</v>
@@ -2698,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="O25" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="P25" t="s">
         <v>30</v>
@@ -2710,16 +2848,16 @@
         <v>45408</v>
       </c>
       <c r="S25" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T25" t="s">
         <v>149</v>
       </c>
       <c r="U25" t="s">
+        <v>146</v>
+      </c>
+      <c r="V25" t="s">
         <v>150</v>
-      </c>
-      <c r="V25" t="s">
-        <v>151</v>
       </c>
       <c r="W25" t="s">
         <v>14</v>
@@ -2733,25 +2871,25 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D26" s="2">
         <v>45406</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="G26" s="3">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H26" s="3">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="I26" t="s">
         <v>5</v>
@@ -2760,10 +2898,10 @@
         <v>6</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="L26" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="M26" t="s">
         <v>9</v>
@@ -2772,7 +2910,7 @@
         <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="P26" t="s">
         <v>30</v>
@@ -2784,16 +2922,16 @@
         <v>45408</v>
       </c>
       <c r="S26" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T26" t="s">
         <v>149</v>
       </c>
       <c r="U26" t="s">
+        <v>146</v>
+      </c>
+      <c r="V26" t="s">
         <v>150</v>
-      </c>
-      <c r="V26" t="s">
-        <v>151</v>
       </c>
       <c r="W26" t="s">
         <v>14</v>
@@ -2807,10 +2945,10 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C27" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D27" s="2">
         <v>45406</v>
@@ -2822,10 +2960,10 @@
         <v>155</v>
       </c>
       <c r="G27" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H27" s="3">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="I27" t="s">
         <v>5</v>
@@ -2834,10 +2972,10 @@
         <v>6</v>
       </c>
       <c r="K27" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="L27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="M27" t="s">
         <v>9</v>
@@ -2846,7 +2984,7 @@
         <v>10</v>
       </c>
       <c r="O27" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="P27" t="s">
         <v>30</v>
@@ -2855,19 +2993,19 @@
         <v>45406</v>
       </c>
       <c r="R27" s="2">
-        <v>45411</v>
+        <v>45408</v>
       </c>
       <c r="S27" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="T27" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="U27" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="V27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="W27" t="s">
         <v>14</v>
@@ -2881,25 +3019,25 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" t="s">
         <v>159</v>
       </c>
-      <c r="C28" t="s">
-        <v>136</v>
-      </c>
-      <c r="D28" s="2">
-        <v>45406</v>
-      </c>
-      <c r="E28" t="s">
-        <v>160</v>
-      </c>
-      <c r="F28" t="s">
-        <v>161</v>
-      </c>
       <c r="G28" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H28" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I28" t="s">
         <v>5</v>
@@ -2908,10 +3046,10 @@
         <v>6</v>
       </c>
       <c r="K28" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="L28" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="M28" t="s">
         <v>9</v>
@@ -2929,19 +3067,19 @@
         <v>45406</v>
       </c>
       <c r="R28" s="2">
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="S28" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="T28" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="U28" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="V28" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="W28" t="s">
         <v>14</v>
@@ -2955,19 +3093,19 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="D29" s="2">
         <v>45406</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="G29" s="3">
         <v>10</v>
@@ -2982,10 +3120,10 @@
         <v>6</v>
       </c>
       <c r="K29" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="L29" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="M29" t="s">
         <v>9</v>
@@ -2994,7 +3132,7 @@
         <v>10</v>
       </c>
       <c r="O29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P29" t="s">
         <v>30</v>
@@ -3003,19 +3141,19 @@
         <v>45406</v>
       </c>
       <c r="R29" s="2">
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="S29" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="T29" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="U29" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="V29" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="W29" t="s">
         <v>14</v>
@@ -3029,25 +3167,25 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D30" s="2">
         <v>45406</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="G30" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H30" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I30" t="s">
         <v>5</v>
@@ -3056,10 +3194,10 @@
         <v>6</v>
       </c>
       <c r="K30" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L30" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="M30" t="s">
         <v>9</v>
@@ -3068,7 +3206,7 @@
         <v>10</v>
       </c>
       <c r="O30" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="P30" t="s">
         <v>30</v>
@@ -3080,16 +3218,16 @@
         <v>45408</v>
       </c>
       <c r="S30" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="U30" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="V30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="W30" t="s">
         <v>14</v>
@@ -3103,25 +3241,25 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D31" s="2">
         <v>45406</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="G31" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H31" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I31" t="s">
         <v>5</v>
@@ -3130,10 +3268,10 @@
         <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L31" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="M31" t="s">
         <v>9</v>
@@ -3142,7 +3280,7 @@
         <v>10</v>
       </c>
       <c r="O31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="P31" t="s">
         <v>30</v>
@@ -3154,16 +3292,16 @@
         <v>45408</v>
       </c>
       <c r="S31" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T31" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="U31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="V31" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="W31" t="s">
         <v>14</v>
@@ -3177,25 +3315,25 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D32" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="G32" s="3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H32" s="3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I32" t="s">
         <v>5</v>
@@ -3204,10 +3342,10 @@
         <v>6</v>
       </c>
       <c r="K32" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="L32" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="M32" t="s">
         <v>9</v>
@@ -3216,28 +3354,28 @@
         <v>10</v>
       </c>
       <c r="O32" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="P32" t="s">
         <v>30</v>
       </c>
       <c r="Q32" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="R32" s="2">
-        <v>45414</v>
+        <v>45408</v>
       </c>
       <c r="S32" t="s">
-        <v>178</v>
+        <v>70</v>
       </c>
       <c r="T32" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="U32" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="V32" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="W32" t="s">
         <v>14</v>
@@ -3251,25 +3389,25 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D33" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="G33" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H33" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
         <v>5</v>
@@ -3278,10 +3416,10 @@
         <v>6</v>
       </c>
       <c r="K33" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="M33" t="s">
         <v>9</v>
@@ -3290,28 +3428,28 @@
         <v>10</v>
       </c>
       <c r="O33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="P33" t="s">
         <v>30</v>
       </c>
       <c r="Q33" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="R33" s="2">
-        <v>45414</v>
+        <v>45408</v>
       </c>
       <c r="S33" t="s">
-        <v>178</v>
+        <v>70</v>
       </c>
       <c r="T33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="U33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="V33" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="W33" t="s">
         <v>14</v>
@@ -3325,25 +3463,25 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D34" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="G34" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I34" t="s">
         <v>5</v>
@@ -3352,10 +3490,10 @@
         <v>6</v>
       </c>
       <c r="K34" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="M34" t="s">
         <v>9</v>
@@ -3364,28 +3502,28 @@
         <v>10</v>
       </c>
       <c r="O34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="P34" t="s">
         <v>30</v>
       </c>
       <c r="Q34" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="R34" s="2">
-        <v>45414</v>
+        <v>45408</v>
       </c>
       <c r="S34" t="s">
-        <v>178</v>
+        <v>70</v>
       </c>
       <c r="T34" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="U34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="V34" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="W34" t="s">
         <v>14</v>
@@ -3396,70 +3534,70 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5</v>
+      </c>
+      <c r="H35" s="3">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" t="s">
+        <v>189</v>
+      </c>
+      <c r="L35" t="s">
         <v>190</v>
       </c>
-      <c r="B35" t="s">
+      <c r="M35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" t="s">
         <v>191</v>
       </c>
-      <c r="C35" t="s">
-        <v>192</v>
-      </c>
-      <c r="D35" s="2">
-        <v>45308</v>
-      </c>
-      <c r="E35" t="s">
-        <v>193</v>
-      </c>
-      <c r="F35" t="s">
-        <v>194</v>
-      </c>
-      <c r="G35" s="3">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>195</v>
-      </c>
-      <c r="K35" t="s">
-        <v>196</v>
-      </c>
-      <c r="L35" t="s">
-        <v>197</v>
-      </c>
-      <c r="M35" t="s">
-        <v>198</v>
-      </c>
-      <c r="N35" t="s">
-        <v>10</v>
-      </c>
-      <c r="O35" t="s">
-        <v>199</v>
-      </c>
       <c r="P35" t="s">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="Q35" s="2">
-        <v>45308</v>
+        <v>45406</v>
       </c>
       <c r="R35" s="2">
-        <v>45309</v>
+        <v>45408</v>
       </c>
       <c r="S35" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T35" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="U35" t="s">
-        <v>201</v>
+        <v>138</v>
       </c>
       <c r="V35" t="s">
-        <v>202</v>
+        <v>139</v>
       </c>
       <c r="W35" t="s">
         <v>14</v>
@@ -3470,70 +3608,70 @@
     </row>
     <row r="36" spans="1:24">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C36" t="s">
-        <v>204</v>
+        <v>66</v>
       </c>
       <c r="D36" s="2">
-        <v>45308</v>
+        <v>45406</v>
       </c>
       <c r="E36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="3">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" t="s">
         <v>193</v>
       </c>
-      <c r="F36" t="s">
+      <c r="L36" t="s">
+        <v>68</v>
+      </c>
+      <c r="M36" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" t="s">
+        <v>10</v>
+      </c>
+      <c r="O36" t="s">
         <v>194</v>
       </c>
-      <c r="G36" s="3">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3">
-        <v>1</v>
-      </c>
-      <c r="I36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" t="s">
-        <v>195</v>
-      </c>
-      <c r="K36" t="s">
-        <v>196</v>
-      </c>
-      <c r="L36" t="s">
-        <v>205</v>
-      </c>
-      <c r="M36" t="s">
-        <v>198</v>
-      </c>
-      <c r="N36" t="s">
-        <v>10</v>
-      </c>
-      <c r="O36" t="s">
-        <v>206</v>
-      </c>
       <c r="P36" t="s">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="Q36" s="2">
-        <v>45308</v>
+        <v>45406</v>
       </c>
       <c r="R36" s="2">
-        <v>45309</v>
+        <v>45408</v>
       </c>
       <c r="S36" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T36" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="U36" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
       <c r="V36" t="s">
-        <v>202</v>
+        <v>73</v>
       </c>
       <c r="W36" t="s">
         <v>14</v>
@@ -3544,70 +3682,70 @@
     </row>
     <row r="37" spans="1:24">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C37" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D37" s="2">
-        <v>45308</v>
+        <v>45406</v>
       </c>
       <c r="E37" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F37" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="G37" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H37" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I37" t="s">
         <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="K37" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L37" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="M37" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="N37" t="s">
         <v>10</v>
       </c>
       <c r="O37" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="P37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R37" s="2">
+        <v>45411</v>
+      </c>
+      <c r="S37" t="s">
+        <v>13</v>
+      </c>
+      <c r="T37" t="s">
         <v>200</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>45308</v>
-      </c>
-      <c r="R37" s="2">
-        <v>45309</v>
-      </c>
-      <c r="S37" t="s">
-        <v>82</v>
-      </c>
-      <c r="T37" t="s">
-        <v>196</v>
       </c>
       <c r="U37" t="s">
         <v>201</v>
       </c>
       <c r="V37" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="W37" t="s">
         <v>14</v>
@@ -3618,52 +3756,52 @@
     </row>
     <row r="38" spans="1:24">
       <c r="A38" t="s">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C38" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E38" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G38" s="3">
+        <v>2</v>
+      </c>
+      <c r="H38" s="3">
+        <v>100</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>6</v>
+      </c>
+      <c r="K38" t="s">
         <v>204</v>
-      </c>
-      <c r="D38" s="2">
-        <v>45406</v>
-      </c>
-      <c r="E38" t="s">
-        <v>212</v>
-      </c>
-      <c r="F38" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="3">
-        <v>1</v>
-      </c>
-      <c r="H38" s="3">
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>5</v>
-      </c>
-      <c r="J38" t="s">
-        <v>195</v>
-      </c>
-      <c r="K38" t="s">
-        <v>196</v>
       </c>
       <c r="L38" t="s">
         <v>205</v>
       </c>
       <c r="M38" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="N38" t="s">
         <v>10</v>
       </c>
       <c r="O38" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="P38" t="s">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="Q38" s="2">
         <v>45406</v>
@@ -3672,16 +3810,16 @@
         <v>45408</v>
       </c>
       <c r="S38" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="T38" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="U38" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="V38" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="W38" t="s">
         <v>14</v>
@@ -3692,49 +3830,49 @@
     </row>
     <row r="39" spans="1:24">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D39" s="2">
         <v>45406</v>
       </c>
       <c r="E39" t="s">
-        <v>216</v>
+        <v>34</v>
       </c>
       <c r="F39" t="s">
-        <v>217</v>
+        <v>35</v>
       </c>
       <c r="G39" s="3">
         <v>2</v>
       </c>
       <c r="H39" s="3">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="I39" t="s">
         <v>5</v>
       </c>
       <c r="J39" t="s">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="K39" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="L39" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="M39" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="N39" t="s">
         <v>10</v>
       </c>
       <c r="O39" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="P39" t="s">
         <v>30</v>
@@ -3743,24 +3881,1134 @@
         <v>45406</v>
       </c>
       <c r="R39" s="2">
+        <v>45411</v>
+      </c>
+      <c r="S39" t="s">
+        <v>13</v>
+      </c>
+      <c r="T39" t="s">
+        <v>212</v>
+      </c>
+      <c r="U39" t="s">
+        <v>213</v>
+      </c>
+      <c r="V39" t="s">
+        <v>214</v>
+      </c>
+      <c r="W39" t="s">
+        <v>14</v>
+      </c>
+      <c r="X39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="3">
+        <v>2</v>
+      </c>
+      <c r="H40" s="3">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" t="s">
+        <v>6</v>
+      </c>
+      <c r="K40" t="s">
+        <v>209</v>
+      </c>
+      <c r="L40" t="s">
+        <v>210</v>
+      </c>
+      <c r="M40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" t="s">
+        <v>211</v>
+      </c>
+      <c r="P40" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R40" s="2">
+        <v>45411</v>
+      </c>
+      <c r="S40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T40" t="s">
+        <v>212</v>
+      </c>
+      <c r="U40" t="s">
+        <v>213</v>
+      </c>
+      <c r="V40" t="s">
+        <v>214</v>
+      </c>
+      <c r="W40" t="s">
+        <v>14</v>
+      </c>
+      <c r="X40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>215</v>
+      </c>
+      <c r="C41" t="s">
+        <v>216</v>
+      </c>
+      <c r="D41" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="3">
+        <v>3</v>
+      </c>
+      <c r="H41" s="3">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J41" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" t="s">
+        <v>217</v>
+      </c>
+      <c r="L41" t="s">
+        <v>218</v>
+      </c>
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" t="s">
+        <v>219</v>
+      </c>
+      <c r="P41" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R41" s="2">
         <v>45408</v>
       </c>
-      <c r="S39" t="s">
-        <v>82</v>
-      </c>
-      <c r="T39" t="s">
-        <v>196</v>
-      </c>
-      <c r="U39" t="s">
-        <v>201</v>
-      </c>
-      <c r="V39" t="s">
-        <v>202</v>
-      </c>
-      <c r="W39" t="s">
-        <v>14</v>
-      </c>
-      <c r="X39" t="s">
+      <c r="S41" t="s">
+        <v>70</v>
+      </c>
+      <c r="T41" t="s">
+        <v>220</v>
+      </c>
+      <c r="U41" t="s">
+        <v>221</v>
+      </c>
+      <c r="V41" t="s">
+        <v>218</v>
+      </c>
+      <c r="W41" t="s">
+        <v>14</v>
+      </c>
+      <c r="X41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>215</v>
+      </c>
+      <c r="C42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="3">
+        <v>5</v>
+      </c>
+      <c r="H42" s="3">
+        <v>250</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" t="s">
+        <v>217</v>
+      </c>
+      <c r="L42" t="s">
+        <v>218</v>
+      </c>
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" t="s">
+        <v>219</v>
+      </c>
+      <c r="P42" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R42" s="2">
+        <v>45408</v>
+      </c>
+      <c r="S42" t="s">
+        <v>70</v>
+      </c>
+      <c r="T42" t="s">
+        <v>220</v>
+      </c>
+      <c r="U42" t="s">
+        <v>221</v>
+      </c>
+      <c r="V42" t="s">
+        <v>218</v>
+      </c>
+      <c r="W42" t="s">
+        <v>14</v>
+      </c>
+      <c r="X42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3">
+        <v>20</v>
+      </c>
+      <c r="I43" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43" t="s">
+        <v>6</v>
+      </c>
+      <c r="K43" t="s">
+        <v>217</v>
+      </c>
+      <c r="L43" t="s">
+        <v>218</v>
+      </c>
+      <c r="M43" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" t="s">
+        <v>219</v>
+      </c>
+      <c r="P43" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R43" s="2">
+        <v>45408</v>
+      </c>
+      <c r="S43" t="s">
+        <v>70</v>
+      </c>
+      <c r="T43" t="s">
+        <v>220</v>
+      </c>
+      <c r="U43" t="s">
+        <v>221</v>
+      </c>
+      <c r="V43" t="s">
+        <v>218</v>
+      </c>
+      <c r="W43" t="s">
+        <v>14</v>
+      </c>
+      <c r="X43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="2">
+        <v>45411</v>
+      </c>
+      <c r="E44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" t="s">
+        <v>224</v>
+      </c>
+      <c r="G44" s="3">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3">
+        <v>2</v>
+      </c>
+      <c r="I44" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" t="s">
+        <v>217</v>
+      </c>
+      <c r="L44" t="s">
+        <v>218</v>
+      </c>
+      <c r="M44" t="s">
+        <v>9</v>
+      </c>
+      <c r="N44" t="s">
+        <v>10</v>
+      </c>
+      <c r="O44" t="s">
+        <v>225</v>
+      </c>
+      <c r="P44" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>45411</v>
+      </c>
+      <c r="R44" s="2">
+        <v>45412</v>
+      </c>
+      <c r="S44" t="s">
+        <v>70</v>
+      </c>
+      <c r="T44" t="s">
+        <v>220</v>
+      </c>
+      <c r="U44" t="s">
+        <v>221</v>
+      </c>
+      <c r="V44" t="s">
+        <v>218</v>
+      </c>
+      <c r="W44" t="s">
+        <v>14</v>
+      </c>
+      <c r="X44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" t="s">
+        <v>216</v>
+      </c>
+      <c r="D45" s="2">
+        <v>45411</v>
+      </c>
+      <c r="E45" t="s">
+        <v>226</v>
+      </c>
+      <c r="F45" t="s">
+        <v>227</v>
+      </c>
+      <c r="G45" s="3">
+        <v>75</v>
+      </c>
+      <c r="H45" s="3">
+        <v>75</v>
+      </c>
+      <c r="I45" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" t="s">
+        <v>217</v>
+      </c>
+      <c r="L45" t="s">
+        <v>218</v>
+      </c>
+      <c r="M45" t="s">
+        <v>9</v>
+      </c>
+      <c r="N45" t="s">
+        <v>10</v>
+      </c>
+      <c r="O45" t="s">
+        <v>225</v>
+      </c>
+      <c r="P45" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>45411</v>
+      </c>
+      <c r="R45" s="2">
+        <v>45412</v>
+      </c>
+      <c r="S45" t="s">
+        <v>70</v>
+      </c>
+      <c r="T45" t="s">
+        <v>220</v>
+      </c>
+      <c r="U45" t="s">
+        <v>221</v>
+      </c>
+      <c r="V45" t="s">
+        <v>218</v>
+      </c>
+      <c r="W45" t="s">
+        <v>14</v>
+      </c>
+      <c r="X45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D46" s="2">
+        <v>45411</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4</v>
+      </c>
+      <c r="H46" s="3">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>5</v>
+      </c>
+      <c r="J46" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" t="s">
+        <v>217</v>
+      </c>
+      <c r="L46" t="s">
+        <v>218</v>
+      </c>
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" t="s">
+        <v>10</v>
+      </c>
+      <c r="O46" t="s">
+        <v>225</v>
+      </c>
+      <c r="P46" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>45411</v>
+      </c>
+      <c r="R46" s="2">
+        <v>45412</v>
+      </c>
+      <c r="S46" t="s">
+        <v>70</v>
+      </c>
+      <c r="T46" t="s">
+        <v>220</v>
+      </c>
+      <c r="U46" t="s">
+        <v>221</v>
+      </c>
+      <c r="V46" t="s">
+        <v>218</v>
+      </c>
+      <c r="W46" t="s">
+        <v>14</v>
+      </c>
+      <c r="X46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" t="s">
+        <v>216</v>
+      </c>
+      <c r="D47" s="2">
+        <v>45411</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" s="3">
+        <v>10</v>
+      </c>
+      <c r="H47" s="3">
+        <v>500</v>
+      </c>
+      <c r="I47" t="s">
+        <v>5</v>
+      </c>
+      <c r="J47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" t="s">
+        <v>217</v>
+      </c>
+      <c r="L47" t="s">
+        <v>218</v>
+      </c>
+      <c r="M47" t="s">
+        <v>9</v>
+      </c>
+      <c r="N47" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" t="s">
+        <v>225</v>
+      </c>
+      <c r="P47" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>45411</v>
+      </c>
+      <c r="R47" s="2">
+        <v>45412</v>
+      </c>
+      <c r="S47" t="s">
+        <v>70</v>
+      </c>
+      <c r="T47" t="s">
+        <v>220</v>
+      </c>
+      <c r="U47" t="s">
+        <v>221</v>
+      </c>
+      <c r="V47" t="s">
+        <v>218</v>
+      </c>
+      <c r="W47" t="s">
+        <v>14</v>
+      </c>
+      <c r="X47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>228</v>
+      </c>
+      <c r="C48" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="2">
+        <v>45413</v>
+      </c>
+      <c r="E48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G48" s="3">
+        <v>5</v>
+      </c>
+      <c r="H48" s="3">
+        <v>5</v>
+      </c>
+      <c r="I48" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" t="s">
+        <v>230</v>
+      </c>
+      <c r="L48" t="s">
+        <v>231</v>
+      </c>
+      <c r="M48" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" t="s">
+        <v>232</v>
+      </c>
+      <c r="P48" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>45413</v>
+      </c>
+      <c r="R48" s="2">
+        <v>45414</v>
+      </c>
+      <c r="S48" t="s">
+        <v>233</v>
+      </c>
+      <c r="T48" t="s">
+        <v>234</v>
+      </c>
+      <c r="U48" t="s">
+        <v>235</v>
+      </c>
+      <c r="V48" t="s">
+        <v>165</v>
+      </c>
+      <c r="W48" t="s">
+        <v>14</v>
+      </c>
+      <c r="X48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>228</v>
+      </c>
+      <c r="C49" t="s">
+        <v>229</v>
+      </c>
+      <c r="D49" s="2">
+        <v>45413</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="3">
+        <v>20</v>
+      </c>
+      <c r="H49" s="3">
+        <v>20</v>
+      </c>
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" t="s">
+        <v>230</v>
+      </c>
+      <c r="L49" t="s">
+        <v>231</v>
+      </c>
+      <c r="M49" t="s">
+        <v>9</v>
+      </c>
+      <c r="N49" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" t="s">
+        <v>232</v>
+      </c>
+      <c r="P49" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>45413</v>
+      </c>
+      <c r="R49" s="2">
+        <v>45414</v>
+      </c>
+      <c r="S49" t="s">
+        <v>233</v>
+      </c>
+      <c r="T49" t="s">
+        <v>234</v>
+      </c>
+      <c r="U49" t="s">
+        <v>235</v>
+      </c>
+      <c r="V49" t="s">
+        <v>165</v>
+      </c>
+      <c r="W49" t="s">
+        <v>14</v>
+      </c>
+      <c r="X49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" s="2">
+        <v>45413</v>
+      </c>
+      <c r="E50" t="s">
+        <v>111</v>
+      </c>
+      <c r="F50" t="s">
+        <v>112</v>
+      </c>
+      <c r="G50" s="3">
+        <v>3</v>
+      </c>
+      <c r="H50" s="3">
+        <v>60</v>
+      </c>
+      <c r="I50" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" t="s">
+        <v>238</v>
+      </c>
+      <c r="L50" t="s">
+        <v>231</v>
+      </c>
+      <c r="M50" t="s">
+        <v>9</v>
+      </c>
+      <c r="N50" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" t="s">
+        <v>239</v>
+      </c>
+      <c r="P50" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>45413</v>
+      </c>
+      <c r="R50" s="2">
+        <v>45414</v>
+      </c>
+      <c r="S50" t="s">
+        <v>233</v>
+      </c>
+      <c r="T50" t="s">
+        <v>234</v>
+      </c>
+      <c r="U50" t="s">
+        <v>235</v>
+      </c>
+      <c r="V50" t="s">
+        <v>165</v>
+      </c>
+      <c r="W50" t="s">
+        <v>14</v>
+      </c>
+      <c r="X50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
+      <c r="A51" t="s">
+        <v>240</v>
+      </c>
+      <c r="B51" t="s">
+        <v>241</v>
+      </c>
+      <c r="C51" t="s">
+        <v>242</v>
+      </c>
+      <c r="D51" s="2">
+        <v>45308</v>
+      </c>
+      <c r="E51" t="s">
+        <v>243</v>
+      </c>
+      <c r="F51" t="s">
+        <v>244</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" t="s">
+        <v>245</v>
+      </c>
+      <c r="K51" t="s">
+        <v>246</v>
+      </c>
+      <c r="L51" t="s">
+        <v>247</v>
+      </c>
+      <c r="M51" t="s">
+        <v>248</v>
+      </c>
+      <c r="N51" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" t="s">
+        <v>249</v>
+      </c>
+      <c r="P51" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>45308</v>
+      </c>
+      <c r="R51" s="2">
+        <v>45309</v>
+      </c>
+      <c r="S51" t="s">
+        <v>70</v>
+      </c>
+      <c r="T51" t="s">
+        <v>246</v>
+      </c>
+      <c r="U51" t="s">
+        <v>251</v>
+      </c>
+      <c r="V51" t="s">
+        <v>252</v>
+      </c>
+      <c r="W51" t="s">
+        <v>14</v>
+      </c>
+      <c r="X51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="A52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" t="s">
+        <v>253</v>
+      </c>
+      <c r="C52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D52" s="2">
+        <v>45308</v>
+      </c>
+      <c r="E52" t="s">
+        <v>243</v>
+      </c>
+      <c r="F52" t="s">
+        <v>244</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>5</v>
+      </c>
+      <c r="J52" t="s">
+        <v>245</v>
+      </c>
+      <c r="K52" t="s">
+        <v>246</v>
+      </c>
+      <c r="L52" t="s">
+        <v>255</v>
+      </c>
+      <c r="M52" t="s">
+        <v>248</v>
+      </c>
+      <c r="N52" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" t="s">
+        <v>256</v>
+      </c>
+      <c r="P52" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>45308</v>
+      </c>
+      <c r="R52" s="2">
+        <v>45309</v>
+      </c>
+      <c r="S52" t="s">
+        <v>70</v>
+      </c>
+      <c r="T52" t="s">
+        <v>246</v>
+      </c>
+      <c r="U52" t="s">
+        <v>251</v>
+      </c>
+      <c r="V52" t="s">
+        <v>252</v>
+      </c>
+      <c r="W52" t="s">
+        <v>14</v>
+      </c>
+      <c r="X52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24">
+      <c r="A53" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" t="s">
+        <v>257</v>
+      </c>
+      <c r="C53" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="2">
+        <v>45308</v>
+      </c>
+      <c r="E53" t="s">
+        <v>243</v>
+      </c>
+      <c r="F53" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>5</v>
+      </c>
+      <c r="J53" t="s">
+        <v>245</v>
+      </c>
+      <c r="K53" t="s">
+        <v>246</v>
+      </c>
+      <c r="L53" t="s">
+        <v>259</v>
+      </c>
+      <c r="M53" t="s">
+        <v>248</v>
+      </c>
+      <c r="N53" t="s">
+        <v>10</v>
+      </c>
+      <c r="O53" t="s">
+        <v>260</v>
+      </c>
+      <c r="P53" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>45308</v>
+      </c>
+      <c r="R53" s="2">
+        <v>45309</v>
+      </c>
+      <c r="S53" t="s">
+        <v>70</v>
+      </c>
+      <c r="T53" t="s">
+        <v>246</v>
+      </c>
+      <c r="U53" t="s">
+        <v>251</v>
+      </c>
+      <c r="V53" t="s">
+        <v>252</v>
+      </c>
+      <c r="W53" t="s">
+        <v>14</v>
+      </c>
+      <c r="X53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24">
+      <c r="A54" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" t="s">
+        <v>254</v>
+      </c>
+      <c r="D54" s="2">
+        <v>45406</v>
+      </c>
+      <c r="E54" t="s">
+        <v>262</v>
+      </c>
+      <c r="F54" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54" s="3">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3">
+        <v>2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>5</v>
+      </c>
+      <c r="J54" t="s">
+        <v>245</v>
+      </c>
+      <c r="K54" t="s">
+        <v>246</v>
+      </c>
+      <c r="L54" t="s">
+        <v>255</v>
+      </c>
+      <c r="M54" t="s">
+        <v>248</v>
+      </c>
+      <c r="N54" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" t="s">
+        <v>264</v>
+      </c>
+      <c r="P54" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>45406</v>
+      </c>
+      <c r="R54" s="2">
+        <v>45408</v>
+      </c>
+      <c r="S54" t="s">
+        <v>70</v>
+      </c>
+      <c r="T54" t="s">
+        <v>246</v>
+      </c>
+      <c r="U54" t="s">
+        <v>251</v>
+      </c>
+      <c r="V54" t="s">
+        <v>252</v>
+      </c>
+      <c r="W54" t="s">
+        <v>14</v>
+      </c>
+      <c r="X54" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>